<commit_message>
changement horaire pour éclipse
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notescours/support/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC324898-A498-384F-9783-D41F09EDFA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87461B7D-E423-3449-B5BE-177D68F2E39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
+    <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="3" r:id="rId1"/>
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F171512-FA2B-6E4F-9860-0C907C2F4F1F}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1147,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1699,8 +1699,8 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E24" s="2" t="str">
-        <f>modele!D24</f>
-        <v>PowerApps</v>
+        <f>modele!D22</f>
+        <v>Excel</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>modele!E24</f>
@@ -1722,7 +1722,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E25" s="2" t="str">
-        <f>modele!D25</f>
+        <f>modele!D24</f>
         <v>PowerApps</v>
       </c>
       <c r="F25" s="2" t="str">
@@ -1745,8 +1745,8 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="2" t="str">
-        <f>modele!D26</f>
-        <v>Excel</v>
+        <f>modele!D25</f>
+        <v>PowerApps</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>modele!E26</f>
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08FFC77-5335-F243-9422-11C9052373E6}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2430,8 +2430,8 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E24" s="2" t="str">
-        <f>modele!D24</f>
-        <v>PowerApps</v>
+        <f>modele!D22</f>
+        <v>Excel</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>modele!E24</f>
@@ -2453,7 +2453,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E25" s="2" t="str">
-        <f>modele!D25</f>
+        <f>modele!D24</f>
         <v>PowerApps</v>
       </c>
       <c r="F25" s="2" t="str">
@@ -2476,8 +2476,8 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="2" t="str">
-        <f>modele!D26</f>
-        <v>Excel</v>
+        <f>modele!D25</f>
+        <v>PowerApps</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>modele!E26</f>

</xml_diff>

<commit_message>
horaire: passer billeterie cours 1
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/support/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE446BB-D85F-3149-863D-AA4B4DE825B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9836302-E07E-714C-8D5B-44E35708243F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
+    <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="3" r:id="rId1"/>
@@ -100,18 +100,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Plan de cours &lt;br/&gt;[Résolution de problèmes](resolution-probleme.md)&lt;br/&gt;[Introduction apprentissage par problème](apprentissage-probleme.md) &lt;br/&gt;[Formation des équipes pour la session](formation-equipes.md)</t>
-  </si>
-  <si>
     <t>Évaluation formative formelle</t>
   </si>
   <si>
     <t>[Niveaux de service](niveaux-service.md)</t>
   </si>
   <si>
-    <t>[Billeterie](billeterie.md) + [niveaux de priorités](niveaux-priorites.md) + [Types d'utilisateurs](types-utilisateurs.md)</t>
-  </si>
-  <si>
     <t>[Comment faire un document d'aide](document-aide.md)</t>
   </si>
   <si>
@@ -296,6 +290,12 @@
   </si>
   <si>
     <t>2025-05-07  15:15</t>
+  </si>
+  <si>
+    <t>[niveaux de priorités](niveaux-priorites.md) &lt;br/&gt; [Types d'utilisateurs](types-utilisateurs.md)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan de cours &lt;br/&gt;[Résolution de problèmes](resolution-probleme.md)&lt;br/&gt;[Introduction apprentissage par problème](apprentissage-probleme.md) &lt;br/&gt;[Formation des équipes pour la session](formation-equipes.md)&lt;br/&gt;[Billeterie](billeterie.md) </t>
   </si>
 </sst>
 </file>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -350,6 +350,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F171512-FA2B-6E4F-9860-0C907C2F4F1F}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -702,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -718,8 +721,8 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
+      <c r="C3" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -742,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -770,7 +773,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -804,7 +807,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -889,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
@@ -1252,11 +1255,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>modele!C2</f>
-        <v>Plan de cours &lt;br/&gt;[Résolution de problèmes](resolution-probleme.md)&lt;br/&gt;[Introduction apprentissage par problème](apprentissage-probleme.md) &lt;br/&gt;[Formation des équipes pour la session](formation-equipes.md)</v>
+        <v xml:space="preserve">Plan de cours &lt;br/&gt;[Résolution de problèmes](resolution-probleme.md)&lt;br/&gt;[Introduction apprentissage par problème](apprentissage-probleme.md) &lt;br/&gt;[Formation des équipes pour la session](formation-equipes.md)&lt;br/&gt;[Billeterie](billeterie.md) </v>
       </c>
       <c r="E2" s="2" t="str">
         <f>modele!D2</f>
@@ -1275,11 +1278,11 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>modele!C3</f>
-        <v>[Billeterie](billeterie.md) + [niveaux de priorités](niveaux-priorites.md) + [Types d'utilisateurs](types-utilisateurs.md)</v>
+        <v>[niveaux de priorités](niveaux-priorites.md) &lt;br/&gt; [Types d'utilisateurs](types-utilisateurs.md)</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>modele!D3</f>
@@ -1298,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>modele!C4</f>
@@ -1321,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>modele!C5</f>
@@ -1344,7 +1347,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>modele!C6</f>
@@ -1367,7 +1370,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>modele!C7</f>
@@ -1390,7 +1393,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>modele!C8</f>
@@ -1413,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>modele!C9</f>
@@ -1436,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>modele!C10</f>
@@ -1459,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>modele!C11</f>
@@ -1482,7 +1485,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>modele!C12</f>
@@ -1505,7 +1508,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>modele!C13</f>
@@ -1528,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>modele!C14</f>
@@ -1551,7 +1554,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>modele!C15</f>
@@ -1574,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>modele!C16</f>
@@ -1597,7 +1600,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>modele!C17</f>
@@ -1620,7 +1623,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>modele!C18</f>
@@ -1643,7 +1646,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="str">
         <f>modele!C19</f>
@@ -1666,7 +1669,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>modele!C20</f>
@@ -1689,7 +1692,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>modele!C21</f>
@@ -1712,7 +1715,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>modele!C22</f>
@@ -1735,7 +1738,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>modele!C23</f>
@@ -1758,7 +1761,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>modele!C24</f>
@@ -1781,7 +1784,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>modele!C25</f>
@@ -1804,7 +1807,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>modele!C26</f>
@@ -1827,7 +1830,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>modele!C27</f>
@@ -1850,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>modele!C28</f>
@@ -1873,7 +1876,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2" t="str">
         <f>modele!C29</f>
@@ -1896,7 +1899,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D30" s="2" t="str">
         <f>modele!C30</f>
@@ -1919,7 +1922,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>modele!C31</f>
@@ -1943,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08FFC77-5335-F243-9422-11C9052373E6}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1983,11 +1986,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>modele!C2</f>
-        <v>Plan de cours &lt;br/&gt;[Résolution de problèmes](resolution-probleme.md)&lt;br/&gt;[Introduction apprentissage par problème](apprentissage-probleme.md) &lt;br/&gt;[Formation des équipes pour la session](formation-equipes.md)</v>
+        <v xml:space="preserve">Plan de cours &lt;br/&gt;[Résolution de problèmes](resolution-probleme.md)&lt;br/&gt;[Introduction apprentissage par problème](apprentissage-probleme.md) &lt;br/&gt;[Formation des équipes pour la session](formation-equipes.md)&lt;br/&gt;[Billeterie](billeterie.md) </v>
       </c>
       <c r="E2" s="2" t="str">
         <f>modele!D2</f>
@@ -2006,11 +2009,11 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>modele!C3</f>
-        <v>[Billeterie](billeterie.md) + [niveaux de priorités](niveaux-priorites.md) + [Types d'utilisateurs](types-utilisateurs.md)</v>
+        <v>[niveaux de priorités](niveaux-priorites.md) &lt;br/&gt; [Types d'utilisateurs](types-utilisateurs.md)</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>modele!D3</f>
@@ -2029,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>modele!C4</f>
@@ -2052,7 +2055,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>modele!C5</f>
@@ -2075,7 +2078,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>modele!C6</f>
@@ -2098,7 +2101,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>modele!C7</f>
@@ -2121,7 +2124,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>modele!C8</f>
@@ -2144,7 +2147,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>modele!C9</f>
@@ -2167,7 +2170,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>modele!C10</f>
@@ -2190,7 +2193,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>modele!C11</f>
@@ -2213,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>modele!C12</f>
@@ -2236,7 +2239,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>modele!C13</f>
@@ -2259,7 +2262,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>modele!C14</f>
@@ -2282,7 +2285,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>modele!C15</f>
@@ -2305,7 +2308,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>modele!C16</f>
@@ -2328,7 +2331,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>modele!C17</f>
@@ -2351,7 +2354,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>modele!C18</f>
@@ -2374,7 +2377,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" s="2" t="str">
         <f>modele!C19</f>
@@ -2397,7 +2400,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>modele!C20</f>
@@ -2420,7 +2423,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>modele!C21</f>
@@ -2443,7 +2446,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>modele!C22</f>
@@ -2466,7 +2469,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>modele!C23</f>
@@ -2489,7 +2492,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>modele!C24</f>
@@ -2512,7 +2515,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>modele!C25</f>
@@ -2535,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>modele!C26</f>
@@ -2558,7 +2561,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>modele!C27</f>
@@ -2581,7 +2584,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>modele!C28</f>
@@ -2604,7 +2607,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2" t="str">
         <f>modele!C29</f>
@@ -2627,7 +2630,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D30" s="2" t="str">
         <f>modele!C30</f>
@@ -2650,7 +2653,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>modele!C31</f>

</xml_diff>

<commit_message>
remplacer outlook par add-in word
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/support/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D77FFC-8D5A-724A-9C01-670EA4BC6B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9F858-8723-954D-A0A8-CDB3D7B7EF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>Évaluation</t>
   </si>
   <si>
-    <t>Comment chiffrer un courriel dans Outlook</t>
-  </si>
-  <si>
     <t>Billets</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>[Niveaux de priorités](niveaux-priorites.md) &lt;br/&gt; [Types d'utilisateurs](types-utilisateurs.md)</t>
+  </si>
+  <si>
+    <t>Comment ajouter un add-on en Word</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -705,13 +705,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -722,13 +722,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -739,13 +739,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -756,13 +756,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -773,13 +773,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -790,13 +790,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -807,13 +807,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -824,13 +824,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -841,13 +841,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -858,13 +858,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -875,13 +875,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -892,13 +892,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -909,13 +909,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -926,13 +926,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -943,13 +943,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -960,13 +960,13 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -977,13 +977,13 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -994,13 +994,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1011,10 +1011,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
@@ -1028,10 +1028,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>3</v>
@@ -1045,10 +1045,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>3</v>
@@ -1062,13 +1062,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1079,13 +1079,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1096,13 +1096,13 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1113,13 +1113,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1130,13 +1130,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1150,10 +1150,10 @@
         <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1164,10 +1164,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -1181,10 +1181,10 @@
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -1198,10 +1198,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -1241,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>modele!C2</f>
@@ -1278,7 +1278,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>modele!C3</f>
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>modele!C4</f>
@@ -1324,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>modele!C5</f>
@@ -1347,7 +1347,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>modele!C6</f>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="F6" s="2" t="str">
         <f>modele!E6</f>
-        <v>Comment chiffrer un courriel dans Outlook</v>
+        <v>Comment ajouter un add-on en Word</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1370,7 +1370,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>modele!C7</f>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="F7" s="2" t="str">
         <f>modele!E7</f>
-        <v>Comment chiffrer un courriel dans Outlook</v>
+        <v>Comment ajouter un add-on en Word</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1393,7 +1393,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>modele!C8</f>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>modele!C9</f>
@@ -1439,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>modele!C10</f>
@@ -1462,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>modele!C11</f>
@@ -1485,7 +1485,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>modele!C12</f>
@@ -1508,7 +1508,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>modele!C13</f>
@@ -1531,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>modele!C14</f>
@@ -1554,7 +1554,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>modele!C15</f>
@@ -1577,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>modele!C16</f>
@@ -1600,7 +1600,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>modele!C17</f>
@@ -1623,7 +1623,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>modele!C18</f>
@@ -1646,7 +1646,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="2" t="str">
         <f>modele!C19</f>
@@ -1669,7 +1669,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>modele!C20</f>
@@ -1692,7 +1692,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>modele!C21</f>
@@ -1715,7 +1715,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>modele!C22</f>
@@ -1738,7 +1738,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>modele!C23</f>
@@ -1761,7 +1761,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>modele!C24</f>
@@ -1784,7 +1784,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>modele!C25</f>
@@ -1807,7 +1807,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>modele!C26</f>
@@ -1830,7 +1830,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>modele!C27</f>
@@ -1853,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>modele!C28</f>
@@ -1876,7 +1876,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="2" t="str">
         <f>modele!C29</f>
@@ -1899,7 +1899,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="2" t="str">
         <f>modele!C30</f>
@@ -1922,7 +1922,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>modele!C31</f>
@@ -1972,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1986,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>modele!C2</f>
@@ -2009,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>modele!C3</f>
@@ -2032,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>modele!C4</f>
@@ -2055,7 +2055,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>modele!C5</f>
@@ -2078,7 +2078,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>modele!C6</f>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="F6" s="2" t="str">
         <f>modele!E6</f>
-        <v>Comment chiffrer un courriel dans Outlook</v>
+        <v>Comment ajouter un add-on en Word</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2101,7 +2101,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>modele!C7</f>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="F7" s="2" t="str">
         <f>modele!E7</f>
-        <v>Comment chiffrer un courriel dans Outlook</v>
+        <v>Comment ajouter un add-on en Word</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2124,7 +2124,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>modele!C8</f>
@@ -2147,7 +2147,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>modele!C9</f>
@@ -2170,7 +2170,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>modele!C10</f>
@@ -2193,7 +2193,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>modele!C11</f>
@@ -2216,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>modele!C12</f>
@@ -2239,7 +2239,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>modele!C13</f>
@@ -2262,7 +2262,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>modele!C14</f>
@@ -2285,7 +2285,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>modele!C15</f>
@@ -2308,7 +2308,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>modele!C16</f>
@@ -2331,7 +2331,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>modele!C17</f>
@@ -2354,7 +2354,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>modele!C18</f>
@@ -2377,7 +2377,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2" t="str">
         <f>modele!C19</f>
@@ -2400,7 +2400,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>modele!C20</f>
@@ -2423,7 +2423,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>modele!C21</f>
@@ -2446,7 +2446,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>modele!C22</f>
@@ -2469,7 +2469,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>modele!C23</f>
@@ -2492,7 +2492,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>modele!C24</f>
@@ -2515,7 +2515,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>modele!C25</f>
@@ -2538,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>modele!C26</f>
@@ -2561,7 +2561,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>modele!C27</f>
@@ -2584,7 +2584,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>modele!C28</f>
@@ -2607,7 +2607,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2" t="str">
         <f>modele!C29</f>
@@ -2630,7 +2630,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="2" t="str">
         <f>modele!C30</f>
@@ -2653,7 +2653,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>modele!C31</f>

</xml_diff>

<commit_message>
changement temporaire horaire - absence
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/support/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9F858-8723-954D-A0A8-CDB3D7B7EF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F1C47A-53CB-9B4A-B0DC-99F37984C2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>Comment ajouter un add-on en Word</t>
+  </si>
+  <si>
+    <t>**Pas de cours - Absence médicale**</t>
   </si>
 </sst>
 </file>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F171512-FA2B-6E4F-9860-0C907C2F4F1F}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1096,7 +1099,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
@@ -1788,7 +1791,7 @@
       </c>
       <c r="D25" s="2" t="str">
         <f>modele!C25</f>
-        <v xml:space="preserve"> </v>
+        <v>**Pas de cours - Absence médicale**</v>
       </c>
       <c r="E25" s="2" t="str">
         <f>modele!D25</f>
@@ -2519,7 +2522,7 @@
       </c>
       <c r="D25" s="2" t="str">
         <f>modele!C25</f>
-        <v xml:space="preserve"> </v>
+        <v>**Pas de cours - Absence médicale**</v>
       </c>
       <c r="E25" s="2" t="str">
         <f>modele!D24</f>

</xml_diff>